<commit_message>
Y-Achse Format für figure 5 angepasst
</commit_message>
<xml_diff>
--- a/Ausarbeitung/Test_Diagramme.xlsx
+++ b/Ausarbeitung/Test_Diagramme.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -162,7 +159,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -569,11 +565,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449529040"/>
-        <c:axId val="449532960"/>
+        <c:axId val="351484632"/>
+        <c:axId val="351483456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449529040"/>
+        <c:axId val="351484632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +612,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449532960"/>
+        <c:crossAx val="351483456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449532960"/>
+        <c:axId val="351483456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +671,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449529040"/>
+        <c:crossAx val="351484632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -689,7 +685,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -809,7 +804,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1088,11 +1082,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449538056"/>
-        <c:axId val="449537664"/>
+        <c:axId val="352280896"/>
+        <c:axId val="352285600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449538056"/>
+        <c:axId val="352280896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1129,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449537664"/>
+        <c:crossAx val="352285600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1143,7 +1137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449537664"/>
+        <c:axId val="352285600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1188,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449538056"/>
+        <c:crossAx val="352280896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1208,7 +1202,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1606,11 +1599,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449537272"/>
-        <c:axId val="449534920"/>
+        <c:axId val="352286384"/>
+        <c:axId val="352287168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449537272"/>
+        <c:axId val="352286384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1653,7 +1646,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449534920"/>
+        <c:crossAx val="352287168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1661,7 +1654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449534920"/>
+        <c:axId val="352287168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1705,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449537272"/>
+        <c:crossAx val="352286384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1846,7 +1839,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2125,11 +2117,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449536096"/>
-        <c:axId val="449536488"/>
+        <c:axId val="352284424"/>
+        <c:axId val="352287560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449536096"/>
+        <c:axId val="352284424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2172,7 +2164,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449536488"/>
+        <c:crossAx val="352287560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2180,7 +2172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449536488"/>
+        <c:axId val="352287560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2223,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449536096"/>
+        <c:crossAx val="352284424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2245,7 +2237,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2365,7 +2356,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2644,11 +2634,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455398128"/>
-        <c:axId val="455396168"/>
+        <c:axId val="352280504"/>
+        <c:axId val="352281288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455398128"/>
+        <c:axId val="352280504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,7 +2681,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455396168"/>
+        <c:crossAx val="352281288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2699,7 +2689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455396168"/>
+        <c:axId val="352281288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,7 +2740,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455398128"/>
+        <c:crossAx val="352280504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2764,7 +2754,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2884,7 +2873,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3163,11 +3151,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455396952"/>
-        <c:axId val="455397344"/>
+        <c:axId val="350432232"/>
+        <c:axId val="353000504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455396952"/>
+        <c:axId val="350432232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3210,7 +3198,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455397344"/>
+        <c:crossAx val="353000504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3218,7 +3206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455397344"/>
+        <c:axId val="353000504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,7 +3257,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455396952"/>
+        <c:crossAx val="350432232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3284,7 +3272,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3404,7 +3391,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3683,11 +3669,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455398520"/>
-        <c:axId val="455399304"/>
+        <c:axId val="353002464"/>
+        <c:axId val="353002856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455398520"/>
+        <c:axId val="353002464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3730,7 +3716,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455399304"/>
+        <c:crossAx val="353002856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3738,7 +3724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455399304"/>
+        <c:axId val="353002856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3775,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455398520"/>
+        <c:crossAx val="353002464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3804,7 +3790,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3924,7 +3909,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4203,11 +4187,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455399696"/>
-        <c:axId val="455397736"/>
+        <c:axId val="352998152"/>
+        <c:axId val="353003640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455399696"/>
+        <c:axId val="352998152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4250,7 +4234,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455397736"/>
+        <c:crossAx val="353003640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4258,7 +4242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455397736"/>
+        <c:axId val="353003640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4309,7 +4293,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455399696"/>
+        <c:crossAx val="352998152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4323,7 +4307,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4443,7 +4426,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4722,11 +4704,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455400088"/>
-        <c:axId val="455400480"/>
+        <c:axId val="352998544"/>
+        <c:axId val="353001680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455400088"/>
+        <c:axId val="352998544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4769,7 +4751,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455400480"/>
+        <c:crossAx val="353001680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4777,7 +4759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455400480"/>
+        <c:axId val="353001680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4828,7 +4810,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455400088"/>
+        <c:crossAx val="352998544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4842,7 +4824,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4962,7 +4943,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5241,11 +5221,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455400872"/>
-        <c:axId val="455401264"/>
+        <c:axId val="353004032"/>
+        <c:axId val="353004424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455400872"/>
+        <c:axId val="353004032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5288,7 +5268,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455401264"/>
+        <c:crossAx val="353004424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5296,7 +5276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455401264"/>
+        <c:axId val="353004424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,7 +5327,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455400872"/>
+        <c:crossAx val="353004032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5361,7 +5341,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5477,7 +5456,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5756,11 +5734,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455402440"/>
-        <c:axId val="455402832"/>
+        <c:axId val="352998936"/>
+        <c:axId val="352999328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455402440"/>
+        <c:axId val="352998936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5803,7 +5781,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455402832"/>
+        <c:crossAx val="352999328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5811,7 +5789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455402832"/>
+        <c:axId val="352999328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5862,7 +5840,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455402440"/>
+        <c:crossAx val="352998936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5876,7 +5854,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6394,11 +6371,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449522768"/>
-        <c:axId val="449533352"/>
+        <c:axId val="351483064"/>
+        <c:axId val="351482672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449522768"/>
+        <c:axId val="351483064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6441,7 +6418,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449533352"/>
+        <c:crossAx val="351482672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6449,7 +6426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449533352"/>
+        <c:axId val="351482672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6500,7 +6477,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449522768"/>
+        <c:crossAx val="351483064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6630,7 +6607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6909,11 +6885,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455393032"/>
-        <c:axId val="455393424"/>
+        <c:axId val="353000112"/>
+        <c:axId val="353000896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455393032"/>
+        <c:axId val="353000112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6956,7 +6932,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455393424"/>
+        <c:crossAx val="353000896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6964,7 +6940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455393424"/>
+        <c:axId val="353000896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7015,7 +6991,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455393032"/>
+        <c:crossAx val="353000112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7029,7 +7005,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7145,7 +7120,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7424,11 +7398,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455404792"/>
-        <c:axId val="455392640"/>
+        <c:axId val="353604616"/>
+        <c:axId val="353605792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455404792"/>
+        <c:axId val="353604616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7471,7 +7445,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455392640"/>
+        <c:crossAx val="353605792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7479,7 +7453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455392640"/>
+        <c:axId val="353605792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7530,7 +7504,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455404792"/>
+        <c:crossAx val="353604616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7544,7 +7518,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8071,11 +8044,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455405968"/>
-        <c:axId val="455407928"/>
+        <c:axId val="353605008"/>
+        <c:axId val="353605400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455405968"/>
+        <c:axId val="353605008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8118,7 +8091,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455407928"/>
+        <c:crossAx val="353605400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8126,7 +8099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455407928"/>
+        <c:axId val="353605400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8177,7 +8150,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455405968"/>
+        <c:crossAx val="353605008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8316,7 +8289,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8595,11 +8567,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455405184"/>
-        <c:axId val="455405576"/>
+        <c:axId val="353609320"/>
+        <c:axId val="353606968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455405184"/>
+        <c:axId val="353609320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8642,7 +8614,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455405576"/>
+        <c:crossAx val="353606968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8650,7 +8622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455405576"/>
+        <c:axId val="353606968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8701,7 +8673,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455405184"/>
+        <c:crossAx val="353609320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8715,7 +8687,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8831,7 +8802,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9110,11 +9080,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="455406752"/>
-        <c:axId val="455407144"/>
+        <c:axId val="353606184"/>
+        <c:axId val="353607360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455406752"/>
+        <c:axId val="353606184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9157,7 +9127,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455407144"/>
+        <c:crossAx val="353607360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9165,7 +9135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455407144"/>
+        <c:axId val="353607360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9216,7 +9186,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455406752"/>
+        <c:crossAx val="353606184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9230,7 +9200,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9346,7 +9315,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9625,11 +9593,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448769144"/>
-        <c:axId val="448764832"/>
+        <c:axId val="353610104"/>
+        <c:axId val="353603832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448769144"/>
+        <c:axId val="353610104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9672,7 +9640,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448764832"/>
+        <c:crossAx val="353603832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9680,7 +9648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448764832"/>
+        <c:axId val="353603832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9731,7 +9699,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448769144"/>
+        <c:crossAx val="353610104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9745,7 +9713,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9870,7 +9837,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10091,11 +10057,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448776984"/>
-        <c:axId val="448774632"/>
+        <c:axId val="353608144"/>
+        <c:axId val="353610888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448776984"/>
+        <c:axId val="353608144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10138,7 +10104,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448774632"/>
+        <c:crossAx val="353610888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10146,7 +10112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448774632"/>
+        <c:axId val="353610888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10197,7 +10163,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448776984"/>
+        <c:crossAx val="353608144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10211,7 +10177,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10327,7 +10292,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10548,11 +10512,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448765616"/>
-        <c:axId val="448767968"/>
+        <c:axId val="353611280"/>
+        <c:axId val="353604224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448765616"/>
+        <c:axId val="353611280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10595,7 +10559,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448767968"/>
+        <c:crossAx val="353604224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10603,7 +10567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448767968"/>
+        <c:axId val="353604224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10654,7 +10618,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448765616"/>
+        <c:crossAx val="353611280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10668,7 +10632,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10784,7 +10747,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11005,11 +10967,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448771888"/>
-        <c:axId val="448768752"/>
+        <c:axId val="374176960"/>
+        <c:axId val="374179312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448771888"/>
+        <c:axId val="374176960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11052,7 +11014,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448768752"/>
+        <c:crossAx val="374179312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11060,7 +11022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448768752"/>
+        <c:axId val="374179312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11111,7 +11073,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448771888"/>
+        <c:crossAx val="374176960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11125,7 +11087,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11287,7 +11248,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Tabelle1!$B$1</c:f>
+              <c:f>Tabelle1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11308,7 +11269,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:f>Tabelle1!$A$11:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -11338,9 +11299,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Tabelle1!$O$59:$O$65</c:f>
+              <c:f>Tabelle1!$O$59:$O$65</c:f>
               <c:numCache>
-                <c:formatCode>0.0E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>-0.11478428466208788</c:v>
@@ -11377,7 +11338,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Tabelle1!$C$1</c:f>
+              <c:f>Tabelle1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11398,7 +11359,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:f>Tabelle1!$A$11:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -11428,9 +11389,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Tabelle1!$P$59:$P$65</c:f>
+              <c:f>Tabelle1!$P$59:$P$65</c:f>
               <c:numCache>
-                <c:formatCode>0.0E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.82121571533791216</c:v>
@@ -11467,7 +11428,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Tabelle1!$D$1</c:f>
+              <c:f>Tabelle1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11488,7 +11449,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:f>Tabelle1!$A$11:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -11518,9 +11479,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Tabelle1!$Q$59:$Q$65</c:f>
+              <c:f>Tabelle1!$Q$59:$Q$65</c:f>
               <c:numCache>
-                <c:formatCode>0.0E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.59421571533791206</c:v>
@@ -11557,7 +11518,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Tabelle1!$E$1</c:f>
+              <c:f>Tabelle1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11578,7 +11539,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:f>Tabelle1!$A$11:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -11608,9 +11569,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Tabelle1!$R$59:$R$65</c:f>
+              <c:f>Tabelle1!$R$59:$R$65</c:f>
               <c:numCache>
-                <c:formatCode>0.0E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>-0.20378428466208789</c:v>
@@ -11652,11 +11613,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="446924520"/>
-        <c:axId val="448610224"/>
+        <c:axId val="374178136"/>
+        <c:axId val="374179704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="446924520"/>
+        <c:axId val="374178136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11699,7 +11660,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448610224"/>
+        <c:crossAx val="374179704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11707,7 +11668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448610224"/>
+        <c:axId val="374179704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11727,7 +11688,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11758,7 +11719,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446924520"/>
+        <c:crossAx val="374178136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12286,11 +12247,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449524728"/>
-        <c:axId val="449531000"/>
+        <c:axId val="351485024"/>
+        <c:axId val="351481496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449524728"/>
+        <c:axId val="351485024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12333,7 +12294,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449531000"/>
+        <c:crossAx val="351481496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12341,7 +12302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449531000"/>
+        <c:axId val="351481496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12392,7 +12353,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449524728"/>
+        <c:crossAx val="351485024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12905,11 +12866,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449528256"/>
-        <c:axId val="449525120"/>
+        <c:axId val="351481104"/>
+        <c:axId val="351486984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449528256"/>
+        <c:axId val="351481104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12952,7 +12913,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449525120"/>
+        <c:crossAx val="351486984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12960,7 +12921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449525120"/>
+        <c:axId val="351486984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13011,7 +12972,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449528256"/>
+        <c:crossAx val="351481104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13141,7 +13102,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13524,11 +13484,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449523552"/>
-        <c:axId val="449530608"/>
+        <c:axId val="351486592"/>
+        <c:axId val="351487376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449523552"/>
+        <c:axId val="351486592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13571,7 +13531,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449530608"/>
+        <c:crossAx val="351487376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13579,7 +13539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449530608"/>
+        <c:axId val="351487376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13630,7 +13590,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449523552"/>
+        <c:crossAx val="351486592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13644,7 +13604,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13760,7 +13719,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14143,11 +14101,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449523944"/>
-        <c:axId val="449529432"/>
+        <c:axId val="351480712"/>
+        <c:axId val="351481888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449523944"/>
+        <c:axId val="351480712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14190,7 +14148,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449529432"/>
+        <c:crossAx val="351481888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14198,7 +14156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449529432"/>
+        <c:axId val="351481888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14249,7 +14207,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449523944"/>
+        <c:crossAx val="351480712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14263,7 +14221,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14383,7 +14340,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14662,11 +14618,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449525512"/>
-        <c:axId val="449532176"/>
+        <c:axId val="352286776"/>
+        <c:axId val="352282072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449525512"/>
+        <c:axId val="352286776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14709,7 +14665,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449532176"/>
+        <c:crossAx val="352282072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14717,7 +14673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449532176"/>
+        <c:axId val="352282072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14768,7 +14724,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449525512"/>
+        <c:crossAx val="352286776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14782,7 +14738,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14902,7 +14857,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15181,11 +15135,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449526688"/>
-        <c:axId val="449531392"/>
+        <c:axId val="352282464"/>
+        <c:axId val="352284816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449526688"/>
+        <c:axId val="352282464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15228,7 +15182,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449531392"/>
+        <c:crossAx val="352284816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15236,7 +15190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449531392"/>
+        <c:axId val="352284816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15287,7 +15241,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449526688"/>
+        <c:crossAx val="352282464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -15302,7 +15256,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15422,7 +15375,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15701,11 +15653,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="449531784"/>
-        <c:axId val="449532568"/>
+        <c:axId val="352283248"/>
+        <c:axId val="352285208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="449531784"/>
+        <c:axId val="352283248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15748,7 +15700,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449532568"/>
+        <c:crossAx val="352285208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15756,7 +15708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449532568"/>
+        <c:axId val="352285208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15807,7 +15759,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449531784"/>
+        <c:crossAx val="352283248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -15822,7 +15774,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31656,7 +31607,7 @@
         <xdr:cNvPr id="5" name="Diagramm 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31692,7 +31643,7 @@
         <xdr:cNvPr id="9" name="Diagramm 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31730,7 +31681,7 @@
         <xdr:cNvPr id="10" name="Diagramm 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31768,7 +31719,7 @@
         <xdr:cNvPr id="13" name="Diagramm 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31806,7 +31757,7 @@
         <xdr:cNvPr id="15" name="Diagramm 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31844,7 +31795,7 @@
         <xdr:cNvPr id="17" name="Diagramm 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31882,7 +31833,7 @@
         <xdr:cNvPr id="12" name="Diagramm 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31920,7 +31871,7 @@
         <xdr:cNvPr id="18" name="Diagramm 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31958,7 +31909,7 @@
         <xdr:cNvPr id="21" name="Diagramm 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31996,7 +31947,7 @@
         <xdr:cNvPr id="22" name="Diagramm 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32034,7 +31985,7 @@
         <xdr:cNvPr id="27" name="Diagramm 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32072,7 +32023,7 @@
         <xdr:cNvPr id="29" name="Diagramm 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32110,7 +32061,7 @@
         <xdr:cNvPr id="32" name="Diagramm 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32148,7 +32099,7 @@
         <xdr:cNvPr id="34" name="Diagramm 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32186,7 +32137,7 @@
         <xdr:cNvPr id="36" name="Diagramm 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32224,7 +32175,7 @@
         <xdr:cNvPr id="26" name="Diagramm 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32262,7 +32213,7 @@
         <xdr:cNvPr id="28" name="Diagramm 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32300,7 +32251,7 @@
         <xdr:cNvPr id="30" name="Diagramm 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32338,7 +32289,7 @@
         <xdr:cNvPr id="39" name="Diagramm 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32376,7 +32327,7 @@
         <xdr:cNvPr id="41" name="Diagramm 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32414,7 +32365,7 @@
         <xdr:cNvPr id="44" name="Diagramm 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32452,7 +32403,7 @@
         <xdr:cNvPr id="46" name="Diagramm 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32490,7 +32441,7 @@
         <xdr:cNvPr id="48" name="Diagramm 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32528,7 +32479,7 @@
         <xdr:cNvPr id="43" name="Diagramm 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32566,7 +32517,7 @@
         <xdr:cNvPr id="50" name="Diagramm 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000032000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32604,7 +32555,7 @@
         <xdr:cNvPr id="49" name="Diagramm 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32642,7 +32593,7 @@
         <xdr:cNvPr id="57" name="Diagramm 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000039000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32680,7 +32631,7 @@
         <xdr:cNvPr id="58" name="Diagramm 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32718,7 +32669,7 @@
         <xdr:cNvPr id="31" name="Diagramm 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32739,167 +32690,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabelle1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Reinhardt</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Chen</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Huang/Langston</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>StdStableSort</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>10000</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>100000</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>1000000</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>10000000</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>100000000</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>1000000000</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="O59">
-            <v>-0.11478428466208788</v>
-          </cell>
-          <cell r="P59">
-            <v>0.82121571533791216</v>
-          </cell>
-          <cell r="Q59">
-            <v>0.59421571533791206</v>
-          </cell>
-          <cell r="R59">
-            <v>-0.20378428466208789</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="O60">
-            <v>-0.6970123795494495</v>
-          </cell>
-          <cell r="P60">
-            <v>-0.31001237954944955</v>
-          </cell>
-          <cell r="Q60">
-            <v>0.14438762045055045</v>
-          </cell>
-          <cell r="R60">
-            <v>-0.5105123795494495</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="O61">
-            <v>-0.76653047443681166</v>
-          </cell>
-          <cell r="P61">
-            <v>-0.74901047443681168</v>
-          </cell>
-          <cell r="Q61">
-            <v>-0.12044047443681163</v>
-          </cell>
-          <cell r="R61">
-            <v>-0.65594047443681158</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="O62">
-            <v>-0.76618856932417301</v>
-          </cell>
-          <cell r="P62">
-            <v>-0.92369156932417307</v>
-          </cell>
-          <cell r="Q62">
-            <v>-0.21293056932417304</v>
-          </cell>
-          <cell r="R62">
-            <v>-0.10882056932417303</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="O63">
-            <v>-0.78343896421153847</v>
-          </cell>
-          <cell r="P63">
-            <v>-0.96450106421153847</v>
-          </cell>
-          <cell r="Q63">
-            <v>-0.22560026421153842</v>
-          </cell>
-          <cell r="R63">
-            <v>-0.5108832642115384</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="O64">
-            <v>-0.7444724590989017</v>
-          </cell>
-          <cell r="P64">
-            <v>-0.98623519909890178</v>
-          </cell>
-          <cell r="Q64">
-            <v>-0.24078321909890174</v>
-          </cell>
-          <cell r="R64">
-            <v>-0.61714966909890179</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="O65">
-            <v>-0.78437487798626326</v>
-          </cell>
-          <cell r="P65">
-            <v>-1.0010840589862633</v>
-          </cell>
-          <cell r="Q65">
-            <v>-0.25125393198626328</v>
-          </cell>
-          <cell r="R65">
-            <v>8.0737800137367245E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33167,8 +32957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K36" zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC56" sqref="AC56"/>
+    <sheetView tabSelected="1" topLeftCell="K34" zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R65" sqref="O59:R65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34353,19 +34143,19 @@
       <c r="N59" s="3">
         <v>1000</v>
       </c>
-      <c r="O59" s="3">
+      <c r="O59" s="2">
         <f>(O49 - (N49*LOG(N49, 2))) / N49</f>
         <v>-0.11478428466208788</v>
       </c>
-      <c r="P59" s="3">
+      <c r="P59" s="2">
         <f>(P49 - (N49*LOG(N49, 2))) / N49</f>
         <v>0.82121571533791216</v>
       </c>
-      <c r="Q59" s="3">
+      <c r="Q59" s="2">
         <f>(Q49 - (N49*LOG(N49, 2))) / N49</f>
         <v>0.59421571533791206</v>
       </c>
-      <c r="R59" s="3">
+      <c r="R59" s="2">
         <f>(R49 - (N49*LOG(N49, 2))) / N49</f>
         <v>-0.20378428466208789</v>
       </c>
@@ -34393,19 +34183,19 @@
       <c r="N60" s="3">
         <v>10000</v>
       </c>
-      <c r="O60" s="3">
+      <c r="O60" s="2">
         <f t="shared" ref="O60:O65" si="16">(O50 - (N50*LOG(N50, 2))) / N50</f>
         <v>-0.6970123795494495</v>
       </c>
-      <c r="P60" s="3">
+      <c r="P60" s="2">
         <f t="shared" ref="P60:P65" si="17">(P50 - (N50*LOG(N50, 2))) / N50</f>
         <v>-0.31001237954944955</v>
       </c>
-      <c r="Q60" s="3">
+      <c r="Q60" s="2">
         <f t="shared" ref="Q60:Q65" si="18">(Q50 - (N50*LOG(N50, 2))) / N50</f>
         <v>0.14438762045055045</v>
       </c>
-      <c r="R60" s="3">
+      <c r="R60" s="2">
         <f t="shared" ref="R60:R65" si="19">(R50 - (N50*LOG(N50, 2))) / N50</f>
         <v>-0.5105123795494495</v>
       </c>
@@ -34433,19 +34223,19 @@
       <c r="N61" s="3">
         <v>100000</v>
       </c>
-      <c r="O61" s="3">
+      <c r="O61" s="2">
         <f t="shared" si="16"/>
         <v>-0.76653047443681166</v>
       </c>
-      <c r="P61" s="3">
+      <c r="P61" s="2">
         <f t="shared" si="17"/>
         <v>-0.74901047443681168</v>
       </c>
-      <c r="Q61" s="3">
+      <c r="Q61" s="2">
         <f t="shared" si="18"/>
         <v>-0.12044047443681163</v>
       </c>
-      <c r="R61" s="3">
+      <c r="R61" s="2">
         <f t="shared" si="19"/>
         <v>-0.65594047443681158</v>
       </c>
@@ -34455,19 +34245,19 @@
       <c r="N62" s="3">
         <v>1000000</v>
       </c>
-      <c r="O62" s="3">
+      <c r="O62" s="2">
         <f t="shared" si="16"/>
         <v>-0.76618856932417301</v>
       </c>
-      <c r="P62" s="3">
+      <c r="P62" s="2">
         <f t="shared" si="17"/>
         <v>-0.92369156932417307</v>
       </c>
-      <c r="Q62" s="3">
+      <c r="Q62" s="2">
         <f t="shared" si="18"/>
         <v>-0.21293056932417304</v>
       </c>
-      <c r="R62" s="3">
+      <c r="R62" s="2">
         <f t="shared" si="19"/>
         <v>-0.10882056932417303</v>
       </c>
@@ -34477,19 +34267,19 @@
       <c r="N63" s="3">
         <v>10000000</v>
       </c>
-      <c r="O63" s="3">
+      <c r="O63" s="2">
         <f t="shared" si="16"/>
         <v>-0.78343896421153847</v>
       </c>
-      <c r="P63" s="3">
+      <c r="P63" s="2">
         <f t="shared" si="17"/>
         <v>-0.96450106421153847</v>
       </c>
-      <c r="Q63" s="3">
+      <c r="Q63" s="2">
         <f t="shared" si="18"/>
         <v>-0.22560026421153842</v>
       </c>
-      <c r="R63" s="3">
+      <c r="R63" s="2">
         <f t="shared" si="19"/>
         <v>-0.5108832642115384</v>
       </c>
@@ -34499,19 +34289,19 @@
       <c r="N64" s="3">
         <v>100000000</v>
       </c>
-      <c r="O64" s="3">
+      <c r="O64" s="2">
         <f t="shared" si="16"/>
         <v>-0.7444724590989017</v>
       </c>
-      <c r="P64" s="3">
+      <c r="P64" s="2">
         <f t="shared" si="17"/>
         <v>-0.98623519909890178</v>
       </c>
-      <c r="Q64" s="3">
+      <c r="Q64" s="2">
         <f t="shared" si="18"/>
         <v>-0.24078321909890174</v>
       </c>
-      <c r="R64" s="3">
+      <c r="R64" s="2">
         <f t="shared" si="19"/>
         <v>-0.61714966909890179</v>
       </c>
@@ -34521,19 +34311,19 @@
       <c r="N65" s="3">
         <v>1000000000</v>
       </c>
-      <c r="O65" s="3">
+      <c r="O65" s="2">
         <f t="shared" si="16"/>
         <v>-0.78437487798626326</v>
       </c>
-      <c r="P65" s="3">
+      <c r="P65" s="2">
         <f t="shared" si="17"/>
         <v>-1.0010840589862633</v>
       </c>
-      <c r="Q65" s="3">
+      <c r="Q65" s="2">
         <f t="shared" si="18"/>
         <v>-0.25125393198626328</v>
       </c>
-      <c r="R65" s="3">
+      <c r="R65" s="2">
         <f t="shared" si="19"/>
         <v>8.0737800137367245E-3</v>
       </c>

</xml_diff>